<commit_message>
dados demograficos actualizados e ultima versao do pbix
</commit_message>
<xml_diff>
--- a/Arquivos/Parte II - O Regresso/Datasets/Dados demográficos concelho.xlsx
+++ b/Arquivos/Parte II - O Regresso/Datasets/Dados demográficos concelho.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Documents\Projectos\UPskill\Projecto Power\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Documents\Projectos\UPskill\Projecto Power\GymTrend-Task-Force\Arquivos\Parte II - O Regresso\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BFD4DA-408E-4B08-BAD9-1262F2826CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF067A1-F760-4B18-971C-80BC5F82AF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E40F6094-EFE4-47A8-A62B-ED4F1E782E4B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>População Residente</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>Valor Metro Quadrado (2022)</t>
+  </si>
+  <si>
+    <t>Setubal</t>
+  </si>
+  <si>
+    <t>Ganho médio mensal Fem (2021)</t>
+  </si>
+  <si>
+    <t>Ganho médio mensal Mas (2021)</t>
   </si>
 </sst>
 </file>
@@ -540,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B99A33-EB61-4EFE-9428-BC0550B6C46A}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,12 +562,14 @@
     <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -575,18 +586,24 @@
         <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="J1" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B2" s="15">
         <v>122547</v>
@@ -597,20 +614,26 @@
       <c r="D2" s="16">
         <v>0.627</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="18">
         <v>1290.7</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="18">
+        <v>1087.8</v>
+      </c>
+      <c r="G2" s="18">
+        <v>1456.4</v>
+      </c>
+      <c r="H2" s="15">
         <v>104.8</v>
       </c>
-      <c r="G2" s="16">
+      <c r="I2" s="16">
         <v>5.5E-2</v>
       </c>
-      <c r="H2" s="18">
+      <c r="J2" s="18">
         <v>830.03</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>7</v>
       </c>
@@ -623,20 +646,26 @@
       <c r="D3" s="14">
         <v>0.64600000000000002</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="19">
         <v>1423.7</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="19">
+        <v>1242.7</v>
+      </c>
+      <c r="G3" s="19">
+        <v>1574.8</v>
+      </c>
+      <c r="H3" s="13">
         <v>118.1</v>
       </c>
-      <c r="G3" s="14">
+      <c r="I3" s="14">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="H3" s="19">
+      <c r="J3" s="19">
         <v>830.03</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>6</v>
       </c>
@@ -649,20 +678,26 @@
       <c r="D4" s="16">
         <v>0.66200000000000003</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="18">
         <v>1080.8</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="18">
+        <v>1019.6</v>
+      </c>
+      <c r="G4" s="18">
+        <v>1129.2</v>
+      </c>
+      <c r="H4" s="15">
         <v>85.9</v>
       </c>
-      <c r="G4" s="16">
+      <c r="I4" s="16">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="H4" s="18">
+      <c r="J4" s="18">
         <v>830.03</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
@@ -675,16 +710,22 @@
       <c r="D5" s="14">
         <v>0.61099999999999999</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="19">
         <v>1095</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="19">
+        <v>1006.8</v>
+      </c>
+      <c r="G5" s="19">
+        <v>1191.7</v>
+      </c>
+      <c r="H5" s="13">
         <v>95.9</v>
       </c>
-      <c r="G5" s="14">
+      <c r="I5" s="14">
         <v>6.2E-2</v>
       </c>
-      <c r="H5" s="19">
+      <c r="J5" s="19">
         <v>725.56</v>
       </c>
     </row>

</xml_diff>